<commit_message>
Updated test4.xlsx with Sample IDs.
</commit_message>
<xml_diff>
--- a/tests/testthat/input_files/test4.xlsx
+++ b/tests/testthat/input_files/test4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Microplate Cycle 1 (0 h)" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="233">
   <si>
     <t>User: USER</t>
   </si>
@@ -684,9 +684,6 @@
     <t>2. Raw Data (448-10/482-10)</t>
   </si>
   <si>
-    <t>X1</t>
-  </si>
-  <si>
     <t>X2</t>
   </si>
   <si>
@@ -720,262 +717,13 @@
     <t>X12</t>
   </si>
   <si>
-    <t>X13</t>
+    <t>3. Sample IDs</t>
   </si>
   <si>
-    <t>X14</t>
+    <t>P</t>
   </si>
   <si>
-    <t>X15</t>
-  </si>
-  <si>
-    <t>X16</t>
-  </si>
-  <si>
-    <t>X17</t>
-  </si>
-  <si>
-    <t>X18</t>
-  </si>
-  <si>
-    <t>X19</t>
-  </si>
-  <si>
-    <t>X20</t>
-  </si>
-  <si>
-    <t>X21</t>
-  </si>
-  <si>
-    <t>X22</t>
-  </si>
-  <si>
-    <t>X23</t>
-  </si>
-  <si>
-    <t>X24</t>
-  </si>
-  <si>
-    <t>X25</t>
-  </si>
-  <si>
-    <t>X26</t>
-  </si>
-  <si>
-    <t>X27</t>
-  </si>
-  <si>
-    <t>X28</t>
-  </si>
-  <si>
-    <t>X29</t>
-  </si>
-  <si>
-    <t>X30</t>
-  </si>
-  <si>
-    <t>X31</t>
-  </si>
-  <si>
-    <t>X32</t>
-  </si>
-  <si>
-    <t>X33</t>
-  </si>
-  <si>
-    <t>X34</t>
-  </si>
-  <si>
-    <t>X35</t>
-  </si>
-  <si>
-    <t>X36</t>
-  </si>
-  <si>
-    <t>X37</t>
-  </si>
-  <si>
-    <t>X38</t>
-  </si>
-  <si>
-    <t>X39</t>
-  </si>
-  <si>
-    <t>X40</t>
-  </si>
-  <si>
-    <t>X41</t>
-  </si>
-  <si>
-    <t>X42</t>
-  </si>
-  <si>
-    <t>X43</t>
-  </si>
-  <si>
-    <t>X44</t>
-  </si>
-  <si>
-    <t>X45</t>
-  </si>
-  <si>
-    <t>X46</t>
-  </si>
-  <si>
-    <t>X47</t>
-  </si>
-  <si>
-    <t>X48</t>
-  </si>
-  <si>
-    <t>X49</t>
-  </si>
-  <si>
-    <t>X50</t>
-  </si>
-  <si>
-    <t>X51</t>
-  </si>
-  <si>
-    <t>X52</t>
-  </si>
-  <si>
-    <t>X53</t>
-  </si>
-  <si>
-    <t>X54</t>
-  </si>
-  <si>
-    <t>X55</t>
-  </si>
-  <si>
-    <t>X56</t>
-  </si>
-  <si>
-    <t>X57</t>
-  </si>
-  <si>
-    <t>X58</t>
-  </si>
-  <si>
-    <t>X59</t>
-  </si>
-  <si>
-    <t>X60</t>
-  </si>
-  <si>
-    <t>X61</t>
-  </si>
-  <si>
-    <t>X62</t>
-  </si>
-  <si>
-    <t>X63</t>
-  </si>
-  <si>
-    <t>X64</t>
-  </si>
-  <si>
-    <t>X65</t>
-  </si>
-  <si>
-    <t>X66</t>
-  </si>
-  <si>
-    <t>X67</t>
-  </si>
-  <si>
-    <t>X68</t>
-  </si>
-  <si>
-    <t>X69</t>
-  </si>
-  <si>
-    <t>X70</t>
-  </si>
-  <si>
-    <t>X71</t>
-  </si>
-  <si>
-    <t>X72</t>
-  </si>
-  <si>
-    <t>X73</t>
-  </si>
-  <si>
-    <t>X74</t>
-  </si>
-  <si>
-    <t>X75</t>
-  </si>
-  <si>
-    <t>X76</t>
-  </si>
-  <si>
-    <t>X77</t>
-  </si>
-  <si>
-    <t>X78</t>
-  </si>
-  <si>
-    <t>X79</t>
-  </si>
-  <si>
-    <t>X80</t>
-  </si>
-  <si>
-    <t>X81</t>
-  </si>
-  <si>
-    <t>X82</t>
-  </si>
-  <si>
-    <t>X83</t>
-  </si>
-  <si>
-    <t>X84</t>
-  </si>
-  <si>
-    <t>X85</t>
-  </si>
-  <si>
-    <t>X86</t>
-  </si>
-  <si>
-    <t>X87</t>
-  </si>
-  <si>
-    <t>X88</t>
-  </si>
-  <si>
-    <t>X89</t>
-  </si>
-  <si>
-    <t>X90</t>
-  </si>
-  <si>
-    <t>X91</t>
-  </si>
-  <si>
-    <t>X92</t>
-  </si>
-  <si>
-    <t>X93</t>
-  </si>
-  <si>
-    <t>X94</t>
-  </si>
-  <si>
-    <t>X95</t>
-  </si>
-  <si>
-    <t>X96</t>
-  </si>
-  <si>
-    <t>3. Layout</t>
-  </si>
-  <si>
-    <t>Plate: BMG LABTECH 96</t>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -1546,8 +1294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:O45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2270,7 +2018,7 @@
         <v>8998</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>212</v>
       </c>
@@ -2311,7 +2059,7 @@
         <v>7870</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>213</v>
       </c>
@@ -2352,13 +2100,12 @@
         <v>8391</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>315</v>
-      </c>
-      <c r="O36" s="17"/>
+        <v>230</v>
+      </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B37" s="8">
         <v>1</v>
       </c>
@@ -2395,53 +2142,49 @@
       <c r="M37" s="8">
         <v>12</v>
       </c>
-      <c r="O37" s="19" t="s">
-        <v>316</v>
-      </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>206</v>
       </c>
       <c r="B38" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="C38" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="D38" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="E38" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="F38" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="F38" s="10" t="s">
+      <c r="G38" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="G38" s="10" t="s">
+      <c r="H38" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="H38" s="10" t="s">
+      <c r="I38" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="I38" s="10" t="s">
+      <c r="J38" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="J38" s="10" t="s">
+      <c r="K38" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="K38" s="10" t="s">
+      <c r="L38" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="L38" s="10" t="s">
+      <c r="M38" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="M38" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="O38" s="20"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>207</v>
       </c>
@@ -2449,283 +2192,283 @@
         <v>231</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="I39" s="12" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="J39" s="12" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="K39" s="12" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="L39" s="12" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="M39" s="13" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>208</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>244</v>
+        <v>219</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>245</v>
+        <v>220</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>246</v>
+        <v>221</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>247</v>
+        <v>222</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>248</v>
+        <v>223</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>249</v>
+        <v>224</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>250</v>
+        <v>225</v>
       </c>
       <c r="J40" s="12" t="s">
-        <v>251</v>
+        <v>226</v>
       </c>
       <c r="K40" s="12" t="s">
-        <v>252</v>
+        <v>227</v>
       </c>
       <c r="L40" s="12" t="s">
-        <v>253</v>
+        <v>228</v>
       </c>
       <c r="M40" s="13" t="s">
-        <v>254</v>
+        <v>229</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>209</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>256</v>
+        <v>219</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>257</v>
+        <v>220</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>258</v>
+        <v>221</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>259</v>
+        <v>222</v>
       </c>
       <c r="G41" s="12" t="s">
-        <v>260</v>
+        <v>223</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>261</v>
+        <v>224</v>
       </c>
       <c r="I41" s="12" t="s">
-        <v>262</v>
+        <v>225</v>
       </c>
       <c r="J41" s="12" t="s">
-        <v>263</v>
+        <v>226</v>
       </c>
       <c r="K41" s="12" t="s">
-        <v>264</v>
+        <v>227</v>
       </c>
       <c r="L41" s="12" t="s">
-        <v>265</v>
+        <v>228</v>
       </c>
       <c r="M41" s="13" t="s">
-        <v>266</v>
+        <v>229</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>210</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>269</v>
+        <v>220</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>270</v>
+        <v>221</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>271</v>
+        <v>222</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>272</v>
+        <v>223</v>
       </c>
       <c r="H42" s="12" t="s">
-        <v>273</v>
+        <v>224</v>
       </c>
       <c r="I42" s="12" t="s">
-        <v>274</v>
+        <v>225</v>
       </c>
       <c r="J42" s="12" t="s">
-        <v>275</v>
+        <v>226</v>
       </c>
       <c r="K42" s="12" t="s">
-        <v>276</v>
+        <v>227</v>
       </c>
       <c r="L42" s="12" t="s">
-        <v>277</v>
+        <v>228</v>
       </c>
       <c r="M42" s="13" t="s">
-        <v>278</v>
+        <v>229</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>211</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>279</v>
+        <v>232</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>280</v>
+        <v>219</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>281</v>
+        <v>220</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>282</v>
+        <v>221</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>283</v>
+        <v>222</v>
       </c>
       <c r="G43" s="12" t="s">
-        <v>284</v>
+        <v>223</v>
       </c>
       <c r="H43" s="12" t="s">
-        <v>285</v>
+        <v>224</v>
       </c>
       <c r="I43" s="12" t="s">
-        <v>286</v>
+        <v>225</v>
       </c>
       <c r="J43" s="12" t="s">
-        <v>287</v>
+        <v>226</v>
       </c>
       <c r="K43" s="12" t="s">
-        <v>288</v>
+        <v>227</v>
       </c>
       <c r="L43" s="12" t="s">
-        <v>289</v>
+        <v>228</v>
       </c>
       <c r="M43" s="13" t="s">
-        <v>290</v>
+        <v>229</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>212</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>291</v>
+        <v>232</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>292</v>
+        <v>219</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>293</v>
+        <v>220</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>294</v>
+        <v>221</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>295</v>
+        <v>222</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>296</v>
+        <v>223</v>
       </c>
       <c r="H44" s="12" t="s">
-        <v>297</v>
+        <v>224</v>
       </c>
       <c r="I44" s="12" t="s">
-        <v>298</v>
+        <v>225</v>
       </c>
       <c r="J44" s="12" t="s">
-        <v>299</v>
+        <v>226</v>
       </c>
       <c r="K44" s="12" t="s">
-        <v>300</v>
+        <v>227</v>
       </c>
       <c r="L44" s="12" t="s">
-        <v>301</v>
+        <v>228</v>
       </c>
       <c r="M44" s="13" t="s">
-        <v>302</v>
+        <v>229</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>213</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>303</v>
+        <v>232</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>304</v>
+        <v>219</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>305</v>
+        <v>220</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>306</v>
+        <v>221</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>307</v>
+        <v>222</v>
       </c>
       <c r="G45" s="15" t="s">
-        <v>308</v>
+        <v>223</v>
       </c>
       <c r="H45" s="15" t="s">
-        <v>309</v>
+        <v>224</v>
       </c>
       <c r="I45" s="15" t="s">
-        <v>310</v>
+        <v>225</v>
       </c>
       <c r="J45" s="15" t="s">
-        <v>311</v>
+        <v>226</v>
       </c>
       <c r="K45" s="15" t="s">
-        <v>312</v>
+        <v>227</v>
       </c>
       <c r="L45" s="15" t="s">
-        <v>313</v>
+        <v>228</v>
       </c>
       <c r="M45" s="16" t="s">
-        <v>314</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -2737,7 +2480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CT142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>